<commit_message>
added cases for checking for registered voters, who have not voted
</commit_message>
<xml_diff>
--- a/Röstkoder.xlsx
+++ b/Röstkoder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Dokument\voting-vg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674EB04E-DE3B-4938-9FDF-233954E4D3EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF406E60-FA30-40C2-A5AC-7F1CD03FCC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -282,69 +282,71 @@
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>111111</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>222222</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>333333</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>444444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
   </sheetData>

</xml_diff>